<commit_message>
pushing before uv changes
</commit_message>
<xml_diff>
--- a/results/TOPSIS-scores.xlsx
+++ b/results/TOPSIS-scores.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Composite + Original Feedstocks" sheetId="1" r:id="rId1"/>
+    <sheet name="Original Feedstocks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -28,130 +28,58 @@
     <t>TOPSIS Score</t>
   </si>
   <si>
-    <t>SRU-DCW, 190°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 190°C, 1hr</t>
-  </si>
-  <si>
     <t>BSG, 190°C, 1hr</t>
   </si>
   <si>
-    <t>DCW-BSG, 190°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-BSG, 190°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 220°C, 1hr</t>
-  </si>
-  <si>
     <t>SRU, 190°C, 1hr</t>
   </si>
   <si>
     <t>BSG, 220°C, 1hr</t>
   </si>
   <si>
-    <t>SRU-BSG, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 250°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 250°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 250°C, 1hr</t>
-  </si>
-  <si>
     <t>BSG, 250°C, 1hr</t>
   </si>
   <si>
     <t>SRU, 220°C, 1hr</t>
   </si>
   <si>
-    <t>SRU-BSG, 250°C, 1hr</t>
-  </si>
-  <si>
     <t>SRU, 250°C, 1hr</t>
   </si>
   <si>
-    <t>DCW-BSG, 190°C, 3hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 190°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 190°C, 3hr</t>
-  </si>
-  <si>
     <t>BSG, 190°C, 3hr</t>
   </si>
   <si>
-    <t>SRU-DCW, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 250°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-BSG, 190°C, 3hr</t>
-  </si>
-  <si>
     <t>BSG, 220°C, 3hr</t>
   </si>
   <si>
+    <t>DCW, 220°C, 1hr</t>
+  </si>
+  <si>
+    <t>DCW, 190°C, 3hr</t>
+  </si>
+  <si>
     <t>SRU, 190°C, 3hr</t>
   </si>
   <si>
     <t>BSG, 250°C, 3hr</t>
   </si>
   <si>
-    <t>SRU-BSG, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 250°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 250°C, 3hr</t>
+    <t>DCW, 250°C, 1hr</t>
+  </si>
+  <si>
+    <t>DCW, 190°C, 1hr</t>
+  </si>
+  <si>
+    <t>DCW, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>DCW, 250°C, 3hr</t>
   </si>
   <si>
     <t>SRU, 220°C, 3hr</t>
   </si>
   <si>
-    <t>DCW, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW, 190°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-BSG, 250°C, 3hr</t>
-  </si>
-  <si>
     <t>SRU, 250°C, 3hr</t>
-  </si>
-  <si>
-    <t>DCW, 250°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW, 190°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>DCW, 250°C, 3hr</t>
   </si>
 </sst>
 </file>
@@ -509,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -534,13 +462,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.0001862263850355757</v>
+        <v>0.0001880437193751001</v>
       </c>
       <c r="C2">
-        <v>0.04738309156193635</v>
+        <v>0.05337922228018754</v>
       </c>
       <c r="D2">
-        <v>0.9214042069394729</v>
+        <v>0.9066122620322559</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -548,13 +476,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.0001883562320618441</v>
+        <v>0.0002577134682679366</v>
       </c>
       <c r="C3">
-        <v>0.04655836313648203</v>
+        <v>0.0325260961894298</v>
       </c>
       <c r="D3">
-        <v>0.9207754092204141</v>
+        <v>0.8534600911911389</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -562,13 +490,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0001880437193751001</v>
+        <v>0.0002474010409449053</v>
       </c>
       <c r="C4">
-        <v>0.05337922228018754</v>
+        <v>0.05330593755316432</v>
       </c>
       <c r="D4">
-        <v>0.9114251952387736</v>
+        <v>0.8522512690731215</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -576,13 +504,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.0001519577906177864</v>
+        <v>0.000268623734777122</v>
       </c>
       <c r="C5">
-        <v>0.06555259820343191</v>
+        <v>0.05944462463173256</v>
       </c>
       <c r="D5">
-        <v>0.9075681754852416</v>
+        <v>0.8273243031273161</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -590,13 +518,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.0002232404174753391</v>
+        <v>0.000334742164809685</v>
       </c>
       <c r="C6">
-        <v>0.04102388232301177</v>
+        <v>0.03588628994357494</v>
       </c>
       <c r="D6">
-        <v>0.8973368509707388</v>
+        <v>0.7817807949065314</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -604,13 +532,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.0002233305936743283</v>
+        <v>0.0003754955726326642</v>
       </c>
       <c r="C7">
-        <v>0.0523876492360877</v>
+        <v>0.039412982896282</v>
       </c>
       <c r="D7">
-        <v>0.8863681208413672</v>
+        <v>0.7445366454910504</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -618,13 +546,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.0002227437412984418</v>
+        <v>0.0004161798657975516</v>
       </c>
       <c r="C8">
-        <v>0.05293577123607186</v>
+        <v>0.089424963187377</v>
       </c>
       <c r="D8">
-        <v>0.8861441831267866</v>
+        <v>0.6678227594787132</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -632,13 +560,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.0001794665505349507</v>
+        <v>0.0004677417854389957</v>
       </c>
       <c r="C9">
-        <v>0.07370605769913149</v>
+        <v>0.09884557812231466</v>
       </c>
       <c r="D9">
-        <v>0.8773218132438865</v>
+        <v>0.6150830295041142</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -646,13 +574,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.0002577134682679366</v>
+        <v>0.0001358532452363411</v>
       </c>
       <c r="C10">
-        <v>0.0325260961894298</v>
+        <v>0.2614696190849936</v>
       </c>
       <c r="D10">
-        <v>0.8725662982460183</v>
+        <v>0.5874969871667608</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -660,13 +588,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.0002474010409449053</v>
+        <v>0.0001371164272798835</v>
       </c>
       <c r="C11">
-        <v>0.05330593755316432</v>
+        <v>0.2664401045097286</v>
       </c>
       <c r="D11">
-        <v>0.8665089354755185</v>
+        <v>0.5811120784170876</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -674,13 +602,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.0002735027400334794</v>
+        <v>0.0005760545882799431</v>
       </c>
       <c r="C12">
-        <v>0.04545543754665177</v>
+        <v>0.06532435782977634</v>
       </c>
       <c r="D12">
-        <v>0.8530544456256275</v>
+        <v>0.5700832427735486</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -688,13 +616,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.0002601217097964387</v>
+        <v>0.0005235349149914908</v>
       </c>
       <c r="C13">
-        <v>0.05805660784852937</v>
+        <v>0.1046053867421573</v>
       </c>
       <c r="D13">
-        <v>0.8510523373750766</v>
+        <v>0.5650907917881749</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -702,13 +630,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.000261491099546579</v>
+        <v>0.0001567059527352144</v>
       </c>
       <c r="C14">
-        <v>0.05829835526756597</v>
+        <v>0.289288538647602</v>
       </c>
       <c r="D14">
-        <v>0.8497068650256839</v>
+        <v>0.5480900490572943</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -716,13 +644,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.0002079992762527498</v>
+        <v>0.0001098535716261584</v>
       </c>
       <c r="C15">
-        <v>0.08151443885217967</v>
+        <v>0.3200145073349393</v>
       </c>
       <c r="D15">
-        <v>0.8462810130332882</v>
+        <v>0.5357413053864908</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -730,13 +658,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>0.000268623734777122</v>
+        <v>0.0001582293526243021</v>
       </c>
       <c r="C16">
-        <v>0.05944462463173256</v>
+        <v>0.3266601454641819</v>
       </c>
       <c r="D16">
-        <v>0.8428460448970443</v>
+        <v>0.5119576569961853</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -744,13 +672,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>0.000334742164809685</v>
+        <v>0.0001875340698927118</v>
       </c>
       <c r="C17">
-        <v>0.03588628994357494</v>
+        <v>0.3277558893490503</v>
       </c>
       <c r="D17">
-        <v>0.8104997617755404</v>
+        <v>0.4987982553552665</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -758,13 +686,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>0.0003281547598237258</v>
+        <v>0.0007191214536902643</v>
       </c>
       <c r="C18">
-        <v>0.04977950544346395</v>
+        <v>0.07335478989294379</v>
       </c>
       <c r="D18">
-        <v>0.806593103459845</v>
+        <v>0.4783960006793526</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -772,349 +700,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>0.0003754955726326642</v>
+        <v>0.0008313695228881577</v>
       </c>
       <c r="C19">
-        <v>0.039412982896282</v>
+        <v>0.08124817280761815</v>
       </c>
       <c r="D19">
-        <v>0.7780352316048221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <v>0.0003047567026191647</v>
-      </c>
-      <c r="C20">
-        <v>0.09397834523287972</v>
-      </c>
-      <c r="D20">
-        <v>0.7639472423412407</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21">
-        <v>0.0002847528573387091</v>
-      </c>
-      <c r="C21">
-        <v>0.1220780699960679</v>
-      </c>
-      <c r="D21">
-        <v>0.7217373705991564</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>0.000425945982300637</v>
-      </c>
-      <c r="C22">
-        <v>0.08180916320314831</v>
-      </c>
-      <c r="D22">
-        <v>0.699641249973511</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23">
-        <v>0.0004305900913045976</v>
-      </c>
-      <c r="C23">
-        <v>0.08131583228592916</v>
-      </c>
-      <c r="D23">
-        <v>0.6971015035258988</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24">
-        <v>0.0004161798657975516</v>
-      </c>
-      <c r="C24">
-        <v>0.089424963187377</v>
-      </c>
-      <c r="D24">
-        <v>0.6957567675783244</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25">
-        <v>0.0004132028246519313</v>
-      </c>
-      <c r="C25">
-        <v>0.09973872054321797</v>
-      </c>
-      <c r="D25">
-        <v>0.6821528293796368</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26">
-        <v>0.0004156414915553534</v>
-      </c>
-      <c r="C26">
-        <v>0.09916645284531209</v>
-      </c>
-      <c r="D26">
-        <v>0.6814249837653252</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27">
-        <v>0.0003558341056147894</v>
-      </c>
-      <c r="C27">
-        <v>0.1326155194854167</v>
-      </c>
-      <c r="D27">
-        <v>0.660164320444859</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28">
-        <v>0.0005101354439564239</v>
-      </c>
-      <c r="C28">
-        <v>0.07792428272113035</v>
-      </c>
-      <c r="D28">
-        <v>0.6485288967541958</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29">
-        <v>0.0004677417854389957</v>
-      </c>
-      <c r="C29">
-        <v>0.09884557812231466</v>
-      </c>
-      <c r="D29">
-        <v>0.6474890112652647</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30">
-        <v>0.0005760545882799431</v>
-      </c>
-      <c r="C30">
-        <v>0.06532435782977634</v>
-      </c>
-      <c r="D30">
-        <v>0.6226371358852563</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31">
-        <v>0.0005235349149914908</v>
-      </c>
-      <c r="C31">
-        <v>0.1046053867421573</v>
-      </c>
-      <c r="D31">
-        <v>0.6034500893935471</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>0.0005551299370823306</v>
-      </c>
-      <c r="C32">
-        <v>0.09161764729516277</v>
-      </c>
-      <c r="D32">
-        <v>0.6029527223542255</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33">
-        <v>0.000517001915718602</v>
-      </c>
-      <c r="C33">
-        <v>0.1103845344384494</v>
-      </c>
-      <c r="D33">
-        <v>0.5985486704775781</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34">
-        <v>0.0005175965647000258</v>
-      </c>
-      <c r="C34">
-        <v>0.1107397670646246</v>
-      </c>
-      <c r="D34">
-        <v>0.5976234213721363</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>0.0007191214536902643</v>
-      </c>
-      <c r="C35">
-        <v>0.07335478989294379</v>
-      </c>
-      <c r="D35">
-        <v>0.5398736184571221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>0.0001358532452363411</v>
-      </c>
-      <c r="C36">
-        <v>0.2614696190849936</v>
-      </c>
-      <c r="D36">
-        <v>0.5266323519874987</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>0.0001371164272798835</v>
-      </c>
-      <c r="C37">
-        <v>0.2664401045097286</v>
-      </c>
-      <c r="D37">
-        <v>0.5196132763438418</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38">
-        <v>0.0007035610543029861</v>
-      </c>
-      <c r="C38">
-        <v>0.1023814495111809</v>
-      </c>
-      <c r="D38">
-        <v>0.5093609530691162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39">
-        <v>0.0008313695228881577</v>
-      </c>
-      <c r="C39">
-        <v>0.08124817280761815</v>
-      </c>
-      <c r="D39">
-        <v>0.4867298440642747</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <v>0.0001567059527352144</v>
-      </c>
-      <c r="C40">
-        <v>0.289288538647602</v>
-      </c>
-      <c r="D40">
-        <v>0.4845164906580468</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>0.0001098535716261584</v>
-      </c>
-      <c r="C41">
-        <v>0.3200145073349393</v>
-      </c>
-      <c r="D41">
-        <v>0.4705048872664693</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42">
-        <v>0.0001582293526243021</v>
-      </c>
-      <c r="C42">
-        <v>0.3266601454641819</v>
-      </c>
-      <c r="D42">
-        <v>0.447071196804459</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43">
-        <v>0.0001875340698927118</v>
-      </c>
-      <c r="C43">
-        <v>0.3277558893490503</v>
-      </c>
-      <c r="D43">
-        <v>0.4345338913509099</v>
+        <v>0.4237490645480737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improving regional scope and cleaning for publication
</commit_message>
<xml_diff>
--- a/results/TOPSIS-scores.xlsx
+++ b/results/TOPSIS-scores.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Original Feedstocks" sheetId="1" r:id="rId1"/>
+    <sheet name="Composite + Original Feedstocks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -28,40 +28,118 @@
     <t>TOPSIS Score</t>
   </si>
   <si>
+    <t>DCW-BSG, 190°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 190°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW-BSG, 190°C, 1hr</t>
+  </si>
+  <si>
     <t>BSG, 190°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-BSG, 190°C, 1hr</t>
+  </si>
+  <si>
+    <t>DCW-BSG, 220°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 220°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW-BSG, 220°C, 1hr</t>
+  </si>
+  <si>
+    <t>DCW-BSG, 250°C, 1hr</t>
+  </si>
+  <si>
     <t>SRU, 190°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-DCW-BSG, 250°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 250°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-BSG, 220°C, 1hr</t>
+  </si>
+  <si>
     <t>BSG, 220°C, 1hr</t>
   </si>
   <si>
     <t>BSG, 250°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-BSG, 250°C, 1hr</t>
+  </si>
+  <si>
     <t>SRU, 220°C, 1hr</t>
   </si>
   <si>
+    <t>DCW-BSG, 190°C, 3hr</t>
+  </si>
+  <si>
     <t>SRU, 250°C, 1hr</t>
   </si>
   <si>
+    <t>DCW-BSG, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 190°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW-BSG, 190°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW-BSG, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>DCW-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
     <t>BSG, 190°C, 3hr</t>
   </si>
   <si>
+    <t>SRU-BSG, 190°C, 3hr</t>
+  </si>
+  <si>
     <t>BSG, 220°C, 3hr</t>
   </si>
   <si>
+    <t>SRU-DCW-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 250°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-BSG, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU, 190°C, 3hr</t>
+  </si>
+  <si>
+    <t>BSG, 250°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
     <t>DCW, 220°C, 1hr</t>
   </si>
   <si>
     <t>DCW, 190°C, 3hr</t>
   </si>
   <si>
-    <t>SRU, 190°C, 3hr</t>
-  </si>
-  <si>
-    <t>BSG, 250°C, 3hr</t>
+    <t>SRU, 250°C, 3hr</t>
   </si>
   <si>
     <t>DCW, 250°C, 1hr</t>
@@ -74,12 +152,6 @@
   </si>
   <si>
     <t>DCW, 250°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU, 250°C, 3hr</t>
   </si>
 </sst>
 </file>
@@ -437,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,13 +534,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.0001880437193751001</v>
+        <v>8.448501609690898E-05</v>
       </c>
       <c r="C2">
-        <v>0.05337922228018754</v>
+        <v>0.03043684375703874</v>
       </c>
       <c r="D2">
-        <v>0.9066122620322559</v>
+        <v>0.9326472871614544</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -476,13 +548,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.0002577134682679366</v>
+        <v>0.0001031994461932442</v>
       </c>
       <c r="C3">
-        <v>0.0325260961894298</v>
+        <v>0.02192868209616805</v>
       </c>
       <c r="D3">
-        <v>0.8534600911911389</v>
+        <v>0.932279257564905</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -490,13 +562,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0002474010409449053</v>
+        <v>0.0001043513488269457</v>
       </c>
       <c r="C4">
-        <v>0.05330593755316432</v>
+        <v>0.02154114384213902</v>
       </c>
       <c r="D4">
-        <v>0.8522512690731215</v>
+        <v>0.9310541994475114</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -504,13 +576,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.000268623734777122</v>
+        <v>0.0001063396305015524</v>
       </c>
       <c r="C5">
-        <v>0.05944462463173256</v>
+        <v>0.03018620772126149</v>
       </c>
       <c r="D5">
-        <v>0.8273243031273161</v>
+        <v>0.9098128486335352</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -518,13 +590,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.000334742164809685</v>
+        <v>0.0001234596005393176</v>
       </c>
       <c r="C6">
-        <v>0.03588628994357494</v>
+        <v>0.01894705796049208</v>
       </c>
       <c r="D6">
-        <v>0.7817807949065314</v>
+        <v>0.9046614982514771</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -532,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.0003754955726326642</v>
+        <v>9.963051981850541E-05</v>
       </c>
       <c r="C7">
-        <v>0.039412982896282</v>
+        <v>0.03417157907251747</v>
       </c>
       <c r="D7">
-        <v>0.7445366454910504</v>
+        <v>0.9044430085109132</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -546,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.0004161798657975516</v>
+        <v>0.0001233051920642406</v>
       </c>
       <c r="C8">
-        <v>0.089424963187377</v>
+        <v>0.02447248569553203</v>
       </c>
       <c r="D8">
-        <v>0.6678227594787132</v>
+        <v>0.8992754866695443</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -560,13 +632,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.0004677417854389957</v>
+        <v>0.0001236081716869846</v>
       </c>
       <c r="C9">
-        <v>0.09884557812231466</v>
+        <v>0.02421479840841841</v>
       </c>
       <c r="D9">
-        <v>0.6150830295041142</v>
+        <v>0.8992238672931649</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -574,13 +646,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.0001358532452363411</v>
+        <v>0.0001153412513086333</v>
       </c>
       <c r="C10">
-        <v>0.2614696190849936</v>
+        <v>0.03774942688593447</v>
       </c>
       <c r="D10">
-        <v>0.5874969871667608</v>
+        <v>0.8755405223934319</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -588,13 +660,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.0001371164272798835</v>
+        <v>0.0001437865642680749</v>
       </c>
       <c r="C11">
-        <v>0.2664401045097286</v>
+        <v>0.01814734655337724</v>
       </c>
       <c r="D11">
-        <v>0.5811120784170876</v>
+        <v>0.8755173750045259</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -602,13 +674,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.0005760545882799431</v>
+        <v>0.0001438665140122485</v>
       </c>
       <c r="C12">
-        <v>0.06532435782977634</v>
+        <v>0.02681561502459924</v>
       </c>
       <c r="D12">
-        <v>0.5700832427735486</v>
+        <v>0.8663219275171443</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -616,13 +688,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.0005235349149914908</v>
+        <v>0.0001446400244290785</v>
       </c>
       <c r="C13">
-        <v>0.1046053867421573</v>
+        <v>0.02693027958529788</v>
       </c>
       <c r="D13">
-        <v>0.5650907917881749</v>
+        <v>0.8650484917387381</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -630,13 +702,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.0001567059527352144</v>
+        <v>0.0001511323656374236</v>
       </c>
       <c r="C14">
-        <v>0.289288538647602</v>
+        <v>0.02097657725035805</v>
       </c>
       <c r="D14">
-        <v>0.5480900490572943</v>
+        <v>0.8631862676153684</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -644,13 +716,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.0001098535716261584</v>
+        <v>0.0001417351999777387</v>
       </c>
       <c r="C15">
-        <v>0.3200145073349393</v>
+        <v>0.03053878710551231</v>
       </c>
       <c r="D15">
-        <v>0.5357413053864908</v>
+        <v>0.8623296304871068</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -658,13 +730,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>0.0001582293526243021</v>
+        <v>0.000154917280283288</v>
       </c>
       <c r="C16">
-        <v>0.3266601454641819</v>
+        <v>0.0342821515122247</v>
       </c>
       <c r="D16">
-        <v>0.5119576569961853</v>
+        <v>0.8364236674755051</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -672,13 +744,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>0.0001875340698927118</v>
+        <v>0.0001812235161287606</v>
       </c>
       <c r="C17">
-        <v>0.3277558893490503</v>
+        <v>0.02295828307893244</v>
       </c>
       <c r="D17">
-        <v>0.4987982553552665</v>
+        <v>0.8194348954979551</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -686,13 +758,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>0.0007191214536902643</v>
+        <v>0.0001878809320935216</v>
       </c>
       <c r="C18">
-        <v>0.07335478989294379</v>
+        <v>0.02014191910305217</v>
       </c>
       <c r="D18">
-        <v>0.4783960006793526</v>
+        <v>0.8131652906305682</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -700,13 +772,349 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>0.0008313695228881577</v>
+        <v>0.0001686248862788909</v>
       </c>
       <c r="C19">
-        <v>0.08124817280761815</v>
+        <v>0.04342593540306544</v>
       </c>
       <c r="D19">
-        <v>0.4237490645480737</v>
+        <v>0.7954905817668663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>0.0002112996982645088</v>
+      </c>
+      <c r="C20">
+        <v>0.02217856081577721</v>
+      </c>
+      <c r="D20">
+        <v>0.7804493841475012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>0.0001576168535620175</v>
+      </c>
+      <c r="C21">
+        <v>0.0564319687823945</v>
+      </c>
+      <c r="D21">
+        <v>0.7665242884589356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>0.00023520661832291</v>
+      </c>
+      <c r="C22">
+        <v>0.03772679799467677</v>
+      </c>
+      <c r="D22">
+        <v>0.7256381889439792</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0.0002377436408143249</v>
+      </c>
+      <c r="C23">
+        <v>0.03749496681022069</v>
+      </c>
+      <c r="D23">
+        <v>0.7229908339882701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0.0002281996137817979</v>
+      </c>
+      <c r="C24">
+        <v>0.04600111946239692</v>
+      </c>
+      <c r="D24">
+        <v>0.7155567012285777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>0.0002295226661244181</v>
+      </c>
+      <c r="C25">
+        <v>0.04573244795178021</v>
+      </c>
+      <c r="D25">
+        <v>0.7146181630943698</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>0.000196758030530607</v>
+      </c>
+      <c r="C26">
+        <v>0.06123958381921436</v>
+      </c>
+      <c r="D26">
+        <v>0.7081635047601104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>0.0002334610523642613</v>
+      </c>
+      <c r="C27">
+        <v>0.05016399813900652</v>
+      </c>
+      <c r="D27">
+        <v>0.6986113063132443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>0.0002814510908387553</v>
+      </c>
+      <c r="C28">
+        <v>0.03590403304335361</v>
+      </c>
+      <c r="D28">
+        <v>0.6745314009936937</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>0.0002639638240774191</v>
+      </c>
+      <c r="C29">
+        <v>0.05578218069574715</v>
+      </c>
+      <c r="D29">
+        <v>0.6482647643422434</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>0.000285339183604001</v>
+      </c>
+      <c r="C30">
+        <v>0.05087805222330753</v>
+      </c>
+      <c r="D30">
+        <v>0.6372341811406291</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>0.0002856864560133999</v>
+      </c>
+      <c r="C31">
+        <v>0.05104519373853537</v>
+      </c>
+      <c r="D31">
+        <v>0.63643462036953</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>0.0003062361408101422</v>
+      </c>
+      <c r="C32">
+        <v>0.04220791644013483</v>
+      </c>
+      <c r="D32">
+        <v>0.6346624866299543</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33">
+        <v>0.000319943916139601</v>
+      </c>
+      <c r="C33">
+        <v>0.03628151096889882</v>
+      </c>
+      <c r="D33">
+        <v>0.632346460248279</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>0.0002966208169868295</v>
+      </c>
+      <c r="C34">
+        <v>0.05926660168822986</v>
+      </c>
+      <c r="D34">
+        <v>0.602982831321567</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>0.0004006902576571894</v>
+      </c>
+      <c r="C35">
+        <v>0.04087285883596017</v>
+      </c>
+      <c r="D35">
+        <v>0.5497691364790782</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36">
+        <v>0.0003879731021169557</v>
+      </c>
+      <c r="C36">
+        <v>0.04714917356183868</v>
+      </c>
+      <c r="D36">
+        <v>0.5464318752194508</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>7.67556972306159E-05</v>
+      </c>
+      <c r="C37">
+        <v>0.1477276665903572</v>
+      </c>
+      <c r="D37">
+        <v>0.5165972259434954</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>7.705723325053621E-05</v>
+      </c>
+      <c r="C38">
+        <v>0.1497350659421356</v>
+      </c>
+      <c r="D38">
+        <v>0.5116155101424769</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39">
+        <v>0.0004623436652129611</v>
+      </c>
+      <c r="C39">
+        <v>0.04518397291884332</v>
+      </c>
+      <c r="D39">
+        <v>0.4978417428473018</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40">
+        <v>8.88529526156138E-05</v>
+      </c>
+      <c r="C40">
+        <v>0.1640278519612318</v>
+      </c>
+      <c r="D40">
+        <v>0.4725306184298454</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>6.152164485705824E-05</v>
+      </c>
+      <c r="C41">
+        <v>0.1792187416205821</v>
+      </c>
+      <c r="D41">
+        <v>0.4628929881787429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>8.933389592788183E-05</v>
+      </c>
+      <c r="C42">
+        <v>0.1844273704890454</v>
+      </c>
+      <c r="D42">
+        <v>0.4365834112819662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>0.0001060036979103792</v>
+      </c>
+      <c r="C43">
+        <v>0.1852641298873376</v>
+      </c>
+      <c r="D43">
+        <v>0.4235172992665859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding CAC acknowledgement, minor visualization improvements
</commit_message>
<xml_diff>
--- a/results/TOPSIS-scores.xlsx
+++ b/results/TOPSIS-scores.xlsx
@@ -28,6 +28,9 @@
     <t>TOPSIS Score</t>
   </si>
   <si>
+    <t>DCW-BSG, 190°C, 1hr</t>
+  </si>
+  <si>
     <t>SRU-DCW, 190°C, 1hr</t>
   </si>
   <si>
@@ -37,39 +40,36 @@
     <t>BSG, 190°C, 1hr</t>
   </si>
   <si>
-    <t>DCW-BSG, 190°C, 1hr</t>
+    <t>DCW-BSG, 220°C, 1hr</t>
   </si>
   <si>
     <t>SRU-BSG, 190°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-DCW, 220°C, 1hr</t>
+  </si>
+  <si>
     <t>SRU-DCW-BSG, 220°C, 1hr</t>
   </si>
   <si>
-    <t>SRU-DCW, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 220°C, 1hr</t>
+    <t>DCW-BSG, 250°C, 1hr</t>
   </si>
   <si>
     <t>SRU, 190°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-DCW-BSG, 250°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 250°C, 1hr</t>
+  </si>
+  <si>
+    <t>SRU-BSG, 220°C, 1hr</t>
+  </si>
+  <si>
     <t>BSG, 220°C, 1hr</t>
   </si>
   <si>
-    <t>SRU-BSG, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 250°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 250°C, 1hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 250°C, 1hr</t>
-  </si>
-  <si>
     <t>BSG, 250°C, 1hr</t>
   </si>
   <si>
@@ -79,12 +79,12 @@
     <t>SRU, 220°C, 1hr</t>
   </si>
   <si>
+    <t>DCW-BSG, 190°C, 3hr</t>
+  </si>
+  <si>
     <t>SRU, 250°C, 1hr</t>
   </si>
   <si>
-    <t>DCW-BSG, 190°C, 3hr</t>
-  </si>
-  <si>
     <t>DCW-BSG, 220°C, 3hr</t>
   </si>
   <si>
@@ -94,49 +94,49 @@
     <t>SRU-DCW-BSG, 190°C, 3hr</t>
   </si>
   <si>
+    <t>SRU-DCW, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW-BSG, 220°C, 3hr</t>
+  </si>
+  <si>
+    <t>DCW-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
     <t>BSG, 190°C, 3hr</t>
   </si>
   <si>
-    <t>SRU-DCW, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>DCW-BSG, 250°C, 3hr</t>
-  </si>
-  <si>
     <t>SRU-BSG, 190°C, 3hr</t>
   </si>
   <si>
     <t>BSG, 220°C, 3hr</t>
   </si>
   <si>
+    <t>SRU-DCW-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-DCW, 250°C, 3hr</t>
+  </si>
+  <si>
+    <t>SRU-BSG, 220°C, 3hr</t>
+  </si>
+  <si>
     <t>SRU, 190°C, 3hr</t>
   </si>
   <si>
-    <t>SRU-BSG, 220°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW-BSG, 250°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-DCW, 250°C, 3hr</t>
-  </si>
-  <si>
     <t>BSG, 250°C, 3hr</t>
   </si>
   <si>
     <t>SRU, 220°C, 3hr</t>
   </si>
   <si>
+    <t>SRU-BSG, 250°C, 3hr</t>
+  </si>
+  <si>
     <t>DCW, 220°C, 1hr</t>
   </si>
   <si>
     <t>DCW, 190°C, 3hr</t>
-  </si>
-  <si>
-    <t>SRU-BSG, 250°C, 3hr</t>
   </si>
   <si>
     <t>SRU, 250°C, 3hr</t>
@@ -534,13 +534,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.0001031994461932442</v>
+        <v>8.448501609690892E-05</v>
       </c>
       <c r="C2">
-        <v>0.02648686201761209</v>
+        <v>0.02955260619987041</v>
       </c>
       <c r="D2">
-        <v>0.9228024542938228</v>
+        <v>0.9359865873120499</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -548,13 +548,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.0001043513488269456</v>
+        <v>0.0001031994461932442</v>
       </c>
       <c r="C3">
-        <v>0.02601876857651982</v>
+        <v>0.02129161984216373</v>
       </c>
       <c r="D3">
-        <v>0.9222457831882204</v>
+        <v>0.9332277539497336</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -562,13 +562,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0001063457716840284</v>
+        <v>0.0001043513488269456</v>
       </c>
       <c r="C4">
-        <v>0.0301879509942915</v>
+        <v>0.02091534017597603</v>
       </c>
       <c r="D4">
-        <v>0.9091436870970913</v>
+        <v>0.9319178319220482</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -576,13 +576,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>8.448501609690892E-05</v>
+        <v>0.0001063396305015524</v>
       </c>
       <c r="C5">
-        <v>0.0367635627763138</v>
+        <v>0.0301862077212615</v>
       </c>
       <c r="D5">
-        <v>0.9080264590427762</v>
+        <v>0.9098993401472105</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -590,13 +590,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.0001234596005393175</v>
+        <v>9.963051981850525E-05</v>
       </c>
       <c r="C6">
-        <v>0.02288546605940118</v>
+        <v>0.0331788416571381</v>
       </c>
       <c r="D6">
-        <v>0.8993915422406563</v>
+        <v>0.9079415651904676</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -604,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.0001236081716869847</v>
+        <v>0.0001234596005393175</v>
       </c>
       <c r="C7">
-        <v>0.02924817923007554</v>
+        <v>0.01839661651589788</v>
       </c>
       <c r="D7">
-        <v>0.8883156691545303</v>
+        <v>0.90516219088774</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -621,10 +621,10 @@
         <v>0.0001233051920642405</v>
       </c>
       <c r="C8">
-        <v>0.02955943038450141</v>
+        <v>0.02376152199831063</v>
       </c>
       <c r="D8">
-        <v>0.8880494741751691</v>
+        <v>0.9005477422330521</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -632,13 +632,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>9.963051981850525E-05</v>
+        <v>0.0001236081716869847</v>
       </c>
       <c r="C9">
-        <v>0.0412746144911213</v>
+        <v>0.02351132092688647</v>
       </c>
       <c r="D9">
-        <v>0.8783763132925287</v>
+        <v>0.9004539122669021</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -646,13 +646,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.0001437927054505509</v>
+        <v>0.0001153412513086332</v>
       </c>
       <c r="C10">
-        <v>0.01814812163390863</v>
+        <v>0.03665274743780992</v>
       </c>
       <c r="D10">
-        <v>0.8729188514773683</v>
+        <v>0.8792392455479809</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -660,13 +660,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.0001417413411602148</v>
+        <v>0.0001437865642680749</v>
       </c>
       <c r="C11">
-        <v>0.03054011030725924</v>
+        <v>0.01814734655337725</v>
       </c>
       <c r="D11">
-        <v>0.8603192220042143</v>
+        <v>0.8758552224094133</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -674,13 +674,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.0001511323656374236</v>
+        <v>0.0001438665140122485</v>
       </c>
       <c r="C12">
-        <v>0.02533684900877395</v>
+        <v>0.02603657978321243</v>
       </c>
       <c r="D12">
-        <v>0.85566695634613</v>
+        <v>0.8678581268794422</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -688,13 +688,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.0001438665140122485</v>
+        <v>0.0001446400244290784</v>
       </c>
       <c r="C13">
-        <v>0.03238961155800975</v>
+        <v>0.02614791316043305</v>
       </c>
       <c r="D13">
-        <v>0.8534827263523233</v>
+        <v>0.8665981854572655</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -702,13 +702,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.0001446400244290784</v>
+        <v>0.0001511323656374236</v>
       </c>
       <c r="C14">
-        <v>0.03252811073384781</v>
+        <v>0.02036717512004288</v>
       </c>
       <c r="D14">
-        <v>0.8521190222077646</v>
+        <v>0.8640439431361743</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -716,13 +716,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.0001153412513086332</v>
+        <v>0.0001417351999777389</v>
       </c>
       <c r="C15">
-        <v>0.04559616746627947</v>
+        <v>0.03053878710551233</v>
       </c>
       <c r="D15">
-        <v>0.8478963531475846</v>
+        <v>0.8625906045108921</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -730,13 +730,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>0.0001549234214657639</v>
+        <v>0.000154917280283288</v>
       </c>
       <c r="C16">
-        <v>0.03428351051457563</v>
+        <v>0.0342821515122247</v>
       </c>
       <c r="D16">
-        <v>0.8342253862485001</v>
+        <v>0.8367088673282241</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -747,10 +747,10 @@
         <v>0.0001812235161287605</v>
       </c>
       <c r="C17">
-        <v>0.02773047980750397</v>
+        <v>0.02229130931816595</v>
       </c>
       <c r="D17">
-        <v>0.8097742629511219</v>
+        <v>0.8206126551605293</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -758,13 +758,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>0.0001878870732759977</v>
+        <v>0.0001878809320935218</v>
       </c>
       <c r="C18">
-        <v>0.02014257747321913</v>
+        <v>0.02014191910305219</v>
       </c>
       <c r="D18">
-        <v>0.8092661536005403</v>
+        <v>0.8136716708619097</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -772,13 +772,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>0.0002113058394469848</v>
+        <v>0.0001686248862788909</v>
       </c>
       <c r="C19">
-        <v>0.02217920541011475</v>
+        <v>0.04216434457107661</v>
       </c>
       <c r="D19">
-        <v>0.7759111975056234</v>
+        <v>0.7992401112331669</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -786,13 +786,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>0.0001686248862788909</v>
+        <v>0.0002112996982645088</v>
       </c>
       <c r="C20">
-        <v>0.05245261680398593</v>
+        <v>0.02217856081577721</v>
       </c>
       <c r="D20">
-        <v>0.7670474289964055</v>
+        <v>0.7810384622407109</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -803,10 +803,10 @@
         <v>0.0001576168535620175</v>
       </c>
       <c r="C21">
-        <v>0.06816213413858876</v>
+        <v>0.05479253249193473</v>
       </c>
       <c r="D21">
-        <v>0.7250316312640738</v>
+        <v>0.7722620584902743</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -817,10 +817,10 @@
         <v>0.0002352066183229098</v>
       </c>
       <c r="C22">
-        <v>0.04556883484693981</v>
+        <v>0.03663077595096925</v>
       </c>
       <c r="D22">
-        <v>0.7040051846281087</v>
+        <v>0.7284397586483141</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -831,10 +831,10 @@
         <v>0.0002377436408143248</v>
       </c>
       <c r="C23">
-        <v>0.04528881434378607</v>
+        <v>0.0364056798222849</v>
       </c>
       <c r="D23">
-        <v>0.7015260256322057</v>
+        <v>0.7257707638892701</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -842,13 +842,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>0.0002334671935467372</v>
+        <v>0.0002281996137817976</v>
       </c>
       <c r="C24">
-        <v>0.05016531770072002</v>
+        <v>0.04466471553611818</v>
       </c>
       <c r="D24">
-        <v>0.6948567396606774</v>
+        <v>0.7193380131460024</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -856,13 +856,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>0.0002281996137817976</v>
+        <v>0.0002295226661244181</v>
       </c>
       <c r="C25">
-        <v>0.05556308849354477</v>
+        <v>0.04440384934993415</v>
       </c>
       <c r="D25">
-        <v>0.6867802662705355</v>
+        <v>0.7183635477130789</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -870,13 +870,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>0.0002295226661244181</v>
+        <v>0.0001967580305306071</v>
       </c>
       <c r="C26">
-        <v>0.0552385698928118</v>
+        <v>0.05946047884924575</v>
       </c>
       <c r="D26">
-        <v>0.6860984541546366</v>
+        <v>0.714141215030089</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -884,13 +884,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>0.0001967580305306071</v>
+        <v>0.0002334610523642612</v>
       </c>
       <c r="C27">
-        <v>0.07396907846636927</v>
+        <v>0.05016399813900651</v>
       </c>
       <c r="D27">
-        <v>0.664560114209979</v>
+        <v>0.6990977964458964</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -901,10 +901,10 @@
         <v>0.000281451090838755</v>
       </c>
       <c r="C28">
-        <v>0.04336718298548695</v>
+        <v>0.03486096515089498</v>
       </c>
       <c r="D28">
-        <v>0.6535562330216591</v>
+        <v>0.6772623958015228</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -912,13 +912,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>0.0002639699652598951</v>
+        <v>0.0002639638240774191</v>
       </c>
       <c r="C29">
-        <v>0.05578347848172883</v>
+        <v>0.05578218069574715</v>
       </c>
       <c r="D29">
-        <v>0.6439079858263373</v>
+        <v>0.6488290147622537</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -926,13 +926,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>0.0003199500573220768</v>
+        <v>0.0002853391836040006</v>
       </c>
       <c r="C30">
-        <v>0.03628220737651315</v>
+        <v>0.04939996583003563</v>
       </c>
       <c r="D30">
-        <v>0.6254696457571444</v>
+        <v>0.641588015514171</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -940,13 +940,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>0.0003062361408101421</v>
+        <v>0.0002856864560133998</v>
       </c>
       <c r="C31">
-        <v>0.05098141575029311</v>
+        <v>0.04956225162479836</v>
       </c>
       <c r="D31">
-        <v>0.608535675778201</v>
+        <v>0.640808540263709</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -954,13 +954,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>0.0002853391836040006</v>
+        <v>0.0003062361408101421</v>
       </c>
       <c r="C32">
-        <v>0.06145375919326657</v>
+        <v>0.04098171094970653</v>
       </c>
       <c r="D32">
-        <v>0.604273132076612</v>
+        <v>0.6380878639634013</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -968,13 +968,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>0.0002856864560133998</v>
+        <v>0.0003199439161396009</v>
       </c>
       <c r="C33">
-        <v>0.0616556433845664</v>
+        <v>0.0362815109688988</v>
       </c>
       <c r="D33">
-        <v>0.603327346873041</v>
+        <v>0.6332374339378908</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -982,13 +982,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>0.0002966269581693053</v>
+        <v>0.0002966208169868294</v>
       </c>
       <c r="C34">
-        <v>0.05926782873297805</v>
+        <v>0.05926660168822983</v>
       </c>
       <c r="D34">
-        <v>0.5978457252025234</v>
+        <v>0.6036478897901137</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -996,13 +996,13 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>0.0004006963988396653</v>
+        <v>0.0004006902576571894</v>
       </c>
       <c r="C35">
-        <v>0.04087348527416181</v>
+        <v>0.04087285883596015</v>
       </c>
       <c r="D35">
-        <v>0.5417612512533786</v>
+        <v>0.5508064093658844</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1010,13 +1010,13 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <v>7.676183841309185E-05</v>
+        <v>0.0003879731021169553</v>
       </c>
       <c r="C36">
-        <v>0.1477394862023211</v>
+        <v>0.04577941688188776</v>
       </c>
       <c r="D36">
-        <v>0.5245199410065331</v>
+        <v>0.5505058690902669</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1024,13 +1024,13 @@
         <v>39</v>
       </c>
       <c r="B37">
-        <v>7.706337443301216E-05</v>
+        <v>7.675569723061589E-05</v>
       </c>
       <c r="C37">
-        <v>0.1497469992847202</v>
+        <v>0.1477276665903572</v>
       </c>
       <c r="D37">
-        <v>0.5196024168272176</v>
+        <v>0.5155701343958176</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1038,13 +1038,13 @@
         <v>40</v>
       </c>
       <c r="B38">
-        <v>0.0003879731021169553</v>
+        <v>7.70572332505362E-05</v>
       </c>
       <c r="C38">
-        <v>0.0569497815190222</v>
+        <v>0.1497350659421356</v>
       </c>
       <c r="D38">
-        <v>0.515524544881983</v>
+        <v>0.5105800302257905</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1052,13 +1052,13 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>0.0004623498063954369</v>
+        <v>0.000462343665212961</v>
       </c>
       <c r="C39">
-        <v>0.04518457308500446</v>
+        <v>0.04518397291884331</v>
       </c>
       <c r="D39">
-        <v>0.4895827748904982</v>
+        <v>0.4989127277824035</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1066,13 +1066,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>8.885909379808974E-05</v>
+        <v>8.885295261561377E-05</v>
       </c>
       <c r="C40">
-        <v>0.1640391889504975</v>
+        <v>0.1640278519612318</v>
       </c>
       <c r="D40">
-        <v>0.4808213565817419</v>
+        <v>0.471456114464761</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1080,13 +1080,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>6.152778603953413E-05</v>
+        <v>6.152164485705817E-05</v>
       </c>
       <c r="C41">
-        <v>0.1792366315030446</v>
+        <v>0.1792187416205819</v>
       </c>
       <c r="D41">
-        <v>0.4713957603449274</v>
+        <v>0.4617895196251031</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1094,13 +1094,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>8.934003711035775E-05</v>
+        <v>8.933389592788179E-05</v>
       </c>
       <c r="C42">
-        <v>0.1844400487913176</v>
+        <v>0.1844273704890453</v>
       </c>
       <c r="D42">
-        <v>0.4449983356276637</v>
+        <v>0.4354934051966901</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1108,13 +1108,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>0.000106009839092855</v>
+        <v>0.0001060036979103791</v>
       </c>
       <c r="C43">
-        <v>0.1852748629169422</v>
+        <v>0.1852641298873374</v>
       </c>
       <c r="D43">
-        <v>0.4318325946437161</v>
+        <v>0.4224408900940265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating README with title; finalizing repo for publication
</commit_message>
<xml_diff>
--- a/results/TOPSIS-scores.xlsx
+++ b/results/TOPSIS-scores.xlsx
@@ -40,10 +40,10 @@
     <t>BSG, 190°C, 1hr</t>
   </si>
   <si>
+    <t>SRU-BSG, 190°C, 1hr</t>
+  </si>
+  <si>
     <t>DCW-BSG, 220°C, 1hr</t>
-  </si>
-  <si>
-    <t>SRU-BSG, 190°C, 1hr</t>
   </si>
   <si>
     <t>SRU-DCW, 220°C, 1hr</t>
@@ -537,10 +537,10 @@
         <v>8.448501609690892E-05</v>
       </c>
       <c r="C2">
-        <v>0.02955260619987041</v>
+        <v>0.03043684375703871</v>
       </c>
       <c r="D2">
-        <v>0.9359865873120499</v>
+        <v>0.9326472871614545</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -551,10 +551,10 @@
         <v>0.0001031994461932442</v>
       </c>
       <c r="C3">
-        <v>0.02129161984216373</v>
+        <v>0.02192868209616805</v>
       </c>
       <c r="D3">
-        <v>0.9332277539497336</v>
+        <v>0.932279257564905</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -565,10 +565,10 @@
         <v>0.0001043513488269456</v>
       </c>
       <c r="C4">
-        <v>0.02091534017597603</v>
+        <v>0.021541143842139</v>
       </c>
       <c r="D4">
-        <v>0.9319178319220482</v>
+        <v>0.9310541994475114</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -582,7 +582,7 @@
         <v>0.0301862077212615</v>
       </c>
       <c r="D5">
-        <v>0.9098993401472105</v>
+        <v>0.909812848633535</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -590,13 +590,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>9.963051981850525E-05</v>
+        <v>0.0001234596005393175</v>
       </c>
       <c r="C6">
-        <v>0.0331788416571381</v>
+        <v>0.01894705796049206</v>
       </c>
       <c r="D6">
-        <v>0.9079415651904676</v>
+        <v>0.904661498251477</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -604,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.0001234596005393175</v>
+        <v>9.963051981850525E-05</v>
       </c>
       <c r="C7">
-        <v>0.01839661651589788</v>
+        <v>0.03417157907251742</v>
       </c>
       <c r="D7">
-        <v>0.90516219088774</v>
+        <v>0.9044430085109134</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -621,10 +621,10 @@
         <v>0.0001233051920642405</v>
       </c>
       <c r="C8">
-        <v>0.02376152199831063</v>
+        <v>0.024472485695532</v>
       </c>
       <c r="D8">
-        <v>0.9005477422330521</v>
+        <v>0.8992754866695443</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -635,10 +635,10 @@
         <v>0.0001236081716869847</v>
       </c>
       <c r="C9">
-        <v>0.02351132092688647</v>
+        <v>0.02421479840841842</v>
       </c>
       <c r="D9">
-        <v>0.9004539122669021</v>
+        <v>0.8992238672931646</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -649,10 +649,10 @@
         <v>0.0001153412513086332</v>
       </c>
       <c r="C10">
-        <v>0.03665274743780992</v>
+        <v>0.03774942688593447</v>
       </c>
       <c r="D10">
-        <v>0.8792392455479809</v>
+        <v>0.8755405223934317</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -666,7 +666,7 @@
         <v>0.01814734655337725</v>
       </c>
       <c r="D11">
-        <v>0.8758552224094133</v>
+        <v>0.8755173750045256</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -677,10 +677,10 @@
         <v>0.0001438665140122485</v>
       </c>
       <c r="C12">
-        <v>0.02603657978321243</v>
+        <v>0.02681561502459924</v>
       </c>
       <c r="D12">
-        <v>0.8678581268794422</v>
+        <v>0.8663219275171441</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -691,10 +691,10 @@
         <v>0.0001446400244290784</v>
       </c>
       <c r="C13">
-        <v>0.02614791316043305</v>
+        <v>0.02693027958529786</v>
       </c>
       <c r="D13">
-        <v>0.8665981854572655</v>
+        <v>0.865048491738738</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -705,10 +705,10 @@
         <v>0.0001511323656374236</v>
       </c>
       <c r="C14">
-        <v>0.02036717512004288</v>
+        <v>0.02097657725035804</v>
       </c>
       <c r="D14">
-        <v>0.8640439431361743</v>
+        <v>0.8631862676153682</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -722,7 +722,7 @@
         <v>0.03053878710551233</v>
       </c>
       <c r="D15">
-        <v>0.8625906045108921</v>
+        <v>0.8623296304871063</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -736,7 +736,7 @@
         <v>0.0342821515122247</v>
       </c>
       <c r="D16">
-        <v>0.8367088673282241</v>
+        <v>0.8364236674755049</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -747,10 +747,10 @@
         <v>0.0001812235161287605</v>
       </c>
       <c r="C17">
-        <v>0.02229130931816595</v>
+        <v>0.02295828307893243</v>
       </c>
       <c r="D17">
-        <v>0.8206126551605293</v>
+        <v>0.819434895497955</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -764,7 +764,7 @@
         <v>0.02014191910305219</v>
       </c>
       <c r="D18">
-        <v>0.8136716708619097</v>
+        <v>0.8131652906305677</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -775,10 +775,10 @@
         <v>0.0001686248862788909</v>
       </c>
       <c r="C19">
-        <v>0.04216434457107661</v>
+        <v>0.04342593540306541</v>
       </c>
       <c r="D19">
-        <v>0.7992401112331669</v>
+        <v>0.7954905817668662</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -792,7 +792,7 @@
         <v>0.02217856081577721</v>
       </c>
       <c r="D20">
-        <v>0.7810384622407109</v>
+        <v>0.7804493841475009</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -803,10 +803,10 @@
         <v>0.0001576168535620175</v>
       </c>
       <c r="C21">
-        <v>0.05479253249193473</v>
+        <v>0.05643196878239449</v>
       </c>
       <c r="D21">
-        <v>0.7722620584902743</v>
+        <v>0.7665242884589353</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -817,10 +817,10 @@
         <v>0.0002352066183229098</v>
       </c>
       <c r="C22">
-        <v>0.03663077595096925</v>
+        <v>0.03772679799467675</v>
       </c>
       <c r="D22">
-        <v>0.7284397586483141</v>
+        <v>0.7256381889439791</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -831,10 +831,10 @@
         <v>0.0002377436408143248</v>
       </c>
       <c r="C23">
-        <v>0.0364056798222849</v>
+        <v>0.03749496681022068</v>
       </c>
       <c r="D23">
-        <v>0.7257707638892701</v>
+        <v>0.7229908339882699</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -845,10 +845,10 @@
         <v>0.0002281996137817976</v>
       </c>
       <c r="C24">
-        <v>0.04466471553611818</v>
+        <v>0.04600111946239686</v>
       </c>
       <c r="D24">
-        <v>0.7193380131460024</v>
+        <v>0.715556701228578</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -859,10 +859,10 @@
         <v>0.0002295226661244181</v>
       </c>
       <c r="C25">
-        <v>0.04440384934993415</v>
+        <v>0.04573244795178021</v>
       </c>
       <c r="D25">
-        <v>0.7183635477130789</v>
+        <v>0.7146181630943693</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -873,10 +873,10 @@
         <v>0.0001967580305306071</v>
       </c>
       <c r="C26">
-        <v>0.05946047884924575</v>
+        <v>0.06123958381921438</v>
       </c>
       <c r="D26">
-        <v>0.714141215030089</v>
+        <v>0.70816350476011</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -890,7 +890,7 @@
         <v>0.05016399813900651</v>
       </c>
       <c r="D27">
-        <v>0.6990977964458964</v>
+        <v>0.6986113063132441</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -901,10 +901,10 @@
         <v>0.000281451090838755</v>
       </c>
       <c r="C28">
-        <v>0.03486096515089498</v>
+        <v>0.03590403304335356</v>
       </c>
       <c r="D28">
-        <v>0.6772623958015228</v>
+        <v>0.6745314009936938</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -918,7 +918,7 @@
         <v>0.05578218069574715</v>
       </c>
       <c r="D29">
-        <v>0.6488290147622537</v>
+        <v>0.6482647643422431</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -929,10 +929,10 @@
         <v>0.0002853391836040006</v>
       </c>
       <c r="C30">
-        <v>0.04939996583003563</v>
+        <v>0.05087805222330746</v>
       </c>
       <c r="D30">
-        <v>0.641588015514171</v>
+        <v>0.6372341811406294</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -943,10 +943,10 @@
         <v>0.0002856864560133998</v>
       </c>
       <c r="C31">
-        <v>0.04956225162479836</v>
+        <v>0.05104519373853536</v>
       </c>
       <c r="D31">
-        <v>0.640808540263709</v>
+        <v>0.6364346203695298</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -957,10 +957,10 @@
         <v>0.0003062361408101421</v>
       </c>
       <c r="C32">
-        <v>0.04098171094970653</v>
+        <v>0.04220791644013482</v>
       </c>
       <c r="D32">
-        <v>0.6380878639634013</v>
+        <v>0.6346624866299541</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -974,7 +974,7 @@
         <v>0.0362815109688988</v>
       </c>
       <c r="D33">
-        <v>0.6332374339378908</v>
+        <v>0.6323464602482788</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -988,7 +988,7 @@
         <v>0.05926660168822983</v>
       </c>
       <c r="D34">
-        <v>0.6036478897901137</v>
+        <v>0.6029828313215668</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1002,7 +1002,7 @@
         <v>0.04087285883596015</v>
       </c>
       <c r="D35">
-        <v>0.5508064093658844</v>
+        <v>0.5497691364790779</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1013,10 +1013,10 @@
         <v>0.0003879731021169553</v>
       </c>
       <c r="C36">
-        <v>0.04577941688188776</v>
+        <v>0.04714917356183863</v>
       </c>
       <c r="D36">
-        <v>0.5505058690902669</v>
+        <v>0.5464318752194508</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1030,7 +1030,7 @@
         <v>0.1477276665903572</v>
       </c>
       <c r="D37">
-        <v>0.5155701343958176</v>
+        <v>0.5165972259434952</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1044,7 +1044,7 @@
         <v>0.1497350659421356</v>
       </c>
       <c r="D38">
-        <v>0.5105800302257905</v>
+        <v>0.5116155101424769</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1058,7 +1058,7 @@
         <v>0.04518397291884331</v>
       </c>
       <c r="D39">
-        <v>0.4989127277824035</v>
+        <v>0.4978417428473015</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1072,7 +1072,7 @@
         <v>0.1640278519612318</v>
       </c>
       <c r="D40">
-        <v>0.471456114464761</v>
+        <v>0.4725306184298453</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1086,7 +1086,7 @@
         <v>0.1792187416205819</v>
       </c>
       <c r="D41">
-        <v>0.4617895196251031</v>
+        <v>0.4628929881787433</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1100,7 +1100,7 @@
         <v>0.1844273704890453</v>
       </c>
       <c r="D42">
-        <v>0.4354934051966901</v>
+        <v>0.4365834112819662</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1114,7 +1114,7 @@
         <v>0.1852641298873374</v>
       </c>
       <c r="D43">
-        <v>0.4224408900940265</v>
+        <v>0.4235172992665862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>